<commit_message>
Updated discharge spreadsheet Created a new section to calculate discharge time Updated icons in Software section Updated 3 x icons in source code with wrong size
</commit_message>
<xml_diff>
--- a/Hardware/Batteries/PiJuice Battery Discharge Levels.xlsx
+++ b/Hardware/Batteries/PiJuice Battery Discharge Levels.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="16">
   <si>
     <t>Battery Size (mAh)</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>/mA</t>
+  </si>
+  <si>
+    <t>hours uptime (theoretical)</t>
   </si>
   <si>
     <t>Idling</t>
@@ -213,7 +216,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -228,6 +231,9 @@
     <col customWidth="1" min="12" max="12" width="20.0"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="H1" s="1"/>
+    </row>
     <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
@@ -244,7 +250,6 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -336,34 +341,34 @@
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7">
         <v>100.0</v>
@@ -390,7 +395,7 @@
         <v>230.0</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M6" s="9">
         <f t="shared" ref="M6:T6" si="1">(($A$7*3.7)/(C6*5))*0.75</f>
@@ -430,7 +435,7 @@
         <v>1300.0</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="7">
         <v>140.0</v>
@@ -457,7 +462,7 @@
         <v>310.0</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M7" s="9">
         <f t="shared" ref="M7:T7" si="2">(($A$7*3.7)/(C7*5))*0.75</f>
@@ -495,7 +500,7 @@
     <row r="8">
       <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>140.0</v>
@@ -522,7 +527,7 @@
         <v>290.0</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M8" s="9">
         <f t="shared" ref="M8:T8" si="3">(($A$7*3.7)/(C8*5))*0.75</f>
@@ -560,7 +565,7 @@
     <row r="9">
       <c r="A9" s="11"/>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>240.0</v>
@@ -587,7 +592,7 @@
         <v>350.0</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M9" s="9">
         <f t="shared" ref="M9:T9" si="4">(($A$7*3.7)/(C9*5))*0.75</f>
@@ -727,34 +732,34 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8"/>
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7">
         <v>100.0</v>
@@ -781,7 +786,7 @@
         <v>230.0</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" ref="M13:T13" si="5">(($A$14*3.7)/(C13*5))*0.75</f>
@@ -821,7 +826,7 @@
         <v>1820.0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="7">
         <v>140.0</v>
@@ -848,7 +853,7 @@
         <v>310.0</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M14" s="12">
         <f t="shared" ref="M14:T14" si="6">(($A$14*3.7)/(C14*5))*0.75</f>
@@ -886,7 +891,7 @@
     <row r="15">
       <c r="A15" s="10"/>
       <c r="B15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="7">
         <v>140.0</v>
@@ -913,7 +918,7 @@
         <v>290.0</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M15" s="12">
         <f t="shared" ref="M15:T15" si="7">(($A$14*3.7)/(C15*5))*0.75</f>
@@ -951,7 +956,7 @@
     <row r="16">
       <c r="A16" s="11"/>
       <c r="B16" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="7">
         <v>240.0</v>
@@ -978,7 +983,7 @@
         <v>350.0</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M16" s="12">
         <f t="shared" ref="M16:T16" si="8">(($A$14*3.7)/(C16*5))*0.75</f>
@@ -1118,34 +1123,34 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8"/>
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" s="7">
         <v>100.0</v>
@@ -1172,7 +1177,7 @@
         <v>230.0</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M20" s="12">
         <f t="shared" ref="M20:T20" si="9">(($A$21*3.7)/(C20*5))*0.75</f>
@@ -1212,7 +1217,7 @@
         <v>2300.0</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="7">
         <v>140.0</v>
@@ -1239,7 +1244,7 @@
         <v>310.0</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M21" s="12">
         <f t="shared" ref="M21:T21" si="10">(($A$21*3.7)/(C21*5))*0.75</f>
@@ -1277,7 +1282,7 @@
     <row r="22">
       <c r="A22" s="10"/>
       <c r="B22" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="7">
         <v>140.0</v>
@@ -1304,7 +1309,7 @@
         <v>290.0</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M22" s="12">
         <f t="shared" ref="M22:T22" si="11">(($A$21*3.7)/(C22*5))*0.75</f>
@@ -1342,7 +1347,7 @@
     <row r="23">
       <c r="A23" s="11"/>
       <c r="B23" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="7">
         <v>240.0</v>
@@ -1369,7 +1374,7 @@
         <v>350.0</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M23" s="12">
         <f t="shared" ref="M23:T23" si="12">(($A$21*3.7)/(C23*5))*0.75</f>
@@ -1509,34 +1514,34 @@
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8"/>
       <c r="B27" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="7">
         <v>100.0</v>
@@ -1563,7 +1568,7 @@
         <v>230.0</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M27" s="14">
         <f t="shared" ref="M27:T27" si="13">(($A$28*3.7)/(C27*5))*0.75</f>
@@ -1603,7 +1608,7 @@
         <v>5000.0</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="7">
         <v>140.0</v>
@@ -1630,7 +1635,7 @@
         <v>310.0</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M28" s="14">
         <f t="shared" ref="M28:T28" si="14">(($A$28*3.7)/(C28*5))*0.75</f>
@@ -1668,7 +1673,7 @@
     <row r="29">
       <c r="A29" s="10"/>
       <c r="B29" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="7">
         <v>140.0</v>
@@ -1695,7 +1700,7 @@
         <v>290.0</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M29" s="14">
         <f t="shared" ref="M29:T29" si="15">(($A$28*3.7)/(C29*5))*0.75</f>
@@ -1733,7 +1738,7 @@
     <row r="30">
       <c r="A30" s="11"/>
       <c r="B30" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" s="7">
         <v>240.0</v>
@@ -1760,7 +1765,7 @@
         <v>350.0</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M30" s="14">
         <f t="shared" ref="M30:T30" si="16">(($A$28*3.7)/(C30*5))*0.75</f>
@@ -1883,34 +1888,34 @@
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8"/>
       <c r="B34" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="7">
         <v>100.0</v>
@@ -1937,7 +1942,7 @@
         <v>230.0</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M34" s="9">
         <f t="shared" ref="M34:T34" si="17">(($A$35*3.7)/(C34*5))*0.75</f>
@@ -1977,7 +1982,7 @@
         <v>12000.0</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" s="7">
         <v>140.0</v>
@@ -2004,7 +2009,7 @@
         <v>310.0</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M35" s="9">
         <f t="shared" ref="M35:T35" si="18">(($A$35*3.7)/(C35*5))*0.75</f>
@@ -2042,7 +2047,7 @@
     <row r="36">
       <c r="A36" s="10"/>
       <c r="B36" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="7">
         <v>140.0</v>
@@ -2069,7 +2074,7 @@
         <v>290.0</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M36" s="9">
         <f t="shared" ref="M36:T36" si="19">(($A$35*3.7)/(C36*5))*0.75</f>
@@ -2107,7 +2112,7 @@
     <row r="37">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37" s="7">
         <v>240.0</v>
@@ -2134,7 +2139,7 @@
         <v>350.0</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M37" s="9">
         <f t="shared" ref="M37:T37" si="20">(($A$35*3.7)/(C37*5))*0.75</f>

</xml_diff>

<commit_message>
update spreadsheet with uptime calculator
update spreadsheet with uptime calculator
</commit_message>
<xml_diff>
--- a/Hardware/Batteries/PiJuice Battery Discharge Levels.xlsx
+++ b/Hardware/Batteries/PiJuice Battery Discharge Levels.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PiSupplyOffice\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="27">
   <si>
     <t>Battery Size (mAh)</t>
   </si>
@@ -60,30 +68,94 @@
   <si>
     <t>Shoot 1080p Video</t>
   </si>
+  <si>
+    <t>Battery Voltage</t>
+  </si>
+  <si>
+    <t>Uptime Calculator</t>
+  </si>
+  <si>
+    <t>Pi Voltage</t>
+  </si>
+  <si>
+    <t>Other Voltage</t>
+  </si>
+  <si>
+    <t>Other Input Voltage</t>
+  </si>
+  <si>
+    <t>Total System Efficiency</t>
+  </si>
+  <si>
+    <t>Pi Current Draw (mA)</t>
+  </si>
+  <si>
+    <t>Other Current Draw (mA)</t>
+  </si>
+  <si>
+    <t>Other Input Current (mA)</t>
+  </si>
+  <si>
+    <t>Approx Uptime (hours)</t>
+  </si>
+  <si>
+    <t>Approx Uptime (mins)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -91,7 +163,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -100,8 +172,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
-    <border/>
+  <borders count="8">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -112,8 +190,11 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -123,6 +204,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -137,6 +219,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -145,6 +228,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -153,98 +239,509 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.0"/>
-    <col customWidth="1" min="2" max="2" width="17.86"/>
-    <col customWidth="1" min="12" max="12" width="20.0"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="17">
+        <v>3.7</v>
+      </c>
+      <c r="D2" s="17">
+        <v>250</v>
+      </c>
+      <c r="E2" s="17">
+        <v>5</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="18">
+        <v>0</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="K2" s="18">
+        <f>((C2*B2)/((D2*E2)+(F2*G2)-(H2*I2)))*0.75</f>
+        <v>2.2199999999999998</v>
+      </c>
+      <c r="L2" s="21">
+        <f>K2*60</f>
+        <v>133.19999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -253,7 +750,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -312,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -365,269 +862,269 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D6" s="7">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E6" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F6" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="G6" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H6" s="7">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="I6" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="J6" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="9">
-        <f t="shared" ref="M6:T6" si="1">(($A$7*3.7)/(C6*5))*0.75</f>
-        <v>7.215</v>
+        <f t="shared" ref="M6:T6" si="0">(($A$7*3.7)/(C6*5))*0.75</f>
+        <v>7.2149999999999999</v>
       </c>
       <c r="N6" s="9">
-        <f t="shared" si="1"/>
-        <v>6.0125</v>
+        <f t="shared" si="0"/>
+        <v>6.0125000000000011</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" si="1"/>
-        <v>7.215</v>
+        <f t="shared" si="0"/>
+        <v>7.2149999999999999</v>
       </c>
       <c r="P6" s="9">
-        <f t="shared" si="1"/>
-        <v>5.153571429</v>
+        <f t="shared" si="0"/>
+        <v>5.1535714285714285</v>
       </c>
       <c r="Q6" s="9">
-        <f t="shared" si="1"/>
-        <v>3.6075</v>
+        <f t="shared" si="0"/>
+        <v>3.6074999999999999</v>
       </c>
       <c r="R6" s="9">
-        <f t="shared" si="1"/>
-        <v>2.004166667</v>
+        <f t="shared" si="0"/>
+        <v>2.0041666666666664</v>
       </c>
       <c r="S6" s="9">
-        <f t="shared" si="1"/>
-        <v>3.136956522</v>
+        <f t="shared" si="0"/>
+        <v>3.1369565217391306</v>
       </c>
       <c r="T6" s="9">
-        <f t="shared" si="1"/>
-        <v>3.136956522</v>
-      </c>
-    </row>
-    <row r="7">
+        <f t="shared" si="0"/>
+        <v>3.1369565217391306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
-        <v>1300.0</v>
+        <v>1300</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D7" s="7">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="E7" s="7">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="F7" s="7">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="G7" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H7" s="7">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="I7" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="J7" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M7" s="9">
-        <f t="shared" ref="M7:T7" si="2">(($A$7*3.7)/(C7*5))*0.75</f>
-        <v>5.153571429</v>
+        <f t="shared" ref="M7:T7" si="1">(($A$7*3.7)/(C7*5))*0.75</f>
+        <v>5.1535714285714285</v>
       </c>
       <c r="N7" s="9">
-        <f t="shared" si="2"/>
-        <v>4.509375</v>
+        <f t="shared" si="1"/>
+        <v>4.5093750000000004</v>
       </c>
       <c r="O7" s="9">
-        <f t="shared" si="2"/>
-        <v>5.55</v>
+        <f t="shared" si="1"/>
+        <v>5.5500000000000007</v>
       </c>
       <c r="P7" s="9">
-        <f t="shared" si="2"/>
-        <v>3.797368421</v>
+        <f t="shared" si="1"/>
+        <v>3.7973684210526315</v>
       </c>
       <c r="Q7" s="9">
-        <f t="shared" si="2"/>
-        <v>3.136956522</v>
+        <f t="shared" si="1"/>
+        <v>3.1369565217391306</v>
       </c>
       <c r="R7" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.80375</v>
       </c>
       <c r="S7" s="9">
-        <f t="shared" si="2"/>
-        <v>2.327419355</v>
+        <f t="shared" si="1"/>
+        <v>2.3274193548387094</v>
       </c>
       <c r="T7" s="9">
-        <f t="shared" si="2"/>
-        <v>2.327419355</v>
-      </c>
-    </row>
-    <row r="8">
+        <f t="shared" si="1"/>
+        <v>2.3274193548387094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D8" s="7">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="E8" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="F8" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="G8" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H8" s="7">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="I8" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="J8" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="9">
-        <f t="shared" ref="M8:T8" si="3">(($A$7*3.7)/(C8*5))*0.75</f>
-        <v>5.153571429</v>
+        <f t="shared" ref="M8:T8" si="2">(($A$7*3.7)/(C8*5))*0.75</f>
+        <v>5.1535714285714285</v>
       </c>
       <c r="N8" s="9">
-        <f t="shared" si="3"/>
-        <v>4.244117647</v>
+        <f t="shared" si="2"/>
+        <v>4.2441176470588236</v>
       </c>
       <c r="O8" s="9">
-        <f t="shared" si="3"/>
-        <v>5.153571429</v>
+        <f t="shared" si="2"/>
+        <v>5.1535714285714285</v>
       </c>
       <c r="P8" s="9">
-        <f t="shared" si="3"/>
-        <v>3.6075</v>
+        <f t="shared" si="2"/>
+        <v>3.6074999999999999</v>
       </c>
       <c r="Q8" s="9">
-        <f t="shared" si="3"/>
-        <v>3.00625</v>
+        <f t="shared" si="2"/>
+        <v>3.0062500000000005</v>
       </c>
       <c r="R8" s="9">
-        <f t="shared" si="3"/>
-        <v>1.717857143</v>
+        <f t="shared" si="2"/>
+        <v>1.7178571428571427</v>
       </c>
       <c r="S8" s="9">
-        <f t="shared" si="3"/>
-        <v>2.487931034</v>
+        <f t="shared" si="2"/>
+        <v>2.4879310344827585</v>
       </c>
       <c r="T8" s="9">
-        <f t="shared" si="3"/>
-        <v>2.487931034</v>
-      </c>
-    </row>
-    <row r="9">
+        <f t="shared" si="2"/>
+        <v>2.4879310344827585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D9" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="E9" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F9" s="7">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="G9" s="7">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H9" s="7">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="I9" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="J9" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M9" s="9">
-        <f t="shared" ref="M9:T9" si="4">(($A$7*3.7)/(C9*5))*0.75</f>
-        <v>3.00625</v>
+        <f t="shared" ref="M9:T9" si="3">(($A$7*3.7)/(C9*5))*0.75</f>
+        <v>3.0062500000000005</v>
       </c>
       <c r="N9" s="9">
-        <f t="shared" si="4"/>
-        <v>3.136956522</v>
+        <f t="shared" si="3"/>
+        <v>3.1369565217391306</v>
       </c>
       <c r="O9" s="9">
-        <f t="shared" si="4"/>
-        <v>3.136956522</v>
+        <f t="shared" si="3"/>
+        <v>3.1369565217391306</v>
       </c>
       <c r="P9" s="9">
-        <f t="shared" si="4"/>
-        <v>2.2546875</v>
+        <f t="shared" si="3"/>
+        <v>2.2546875000000002</v>
       </c>
       <c r="Q9" s="9">
-        <f t="shared" si="4"/>
-        <v>2.186363636</v>
+        <f t="shared" si="3"/>
+        <v>2.1863636363636365</v>
       </c>
       <c r="R9" s="9">
-        <f t="shared" si="4"/>
-        <v>1.503125</v>
+        <f t="shared" si="3"/>
+        <v>1.5031250000000003</v>
       </c>
       <c r="S9" s="9">
-        <f t="shared" si="4"/>
-        <v>2.061428571</v>
+        <f t="shared" si="3"/>
+        <v>2.0614285714285714</v>
       </c>
       <c r="T9" s="9">
-        <f t="shared" si="4"/>
-        <v>2.061428571</v>
-      </c>
-    </row>
-    <row r="10">
+        <f t="shared" si="3"/>
+        <v>2.0614285714285714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -644,7 +1141,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -703,7 +1200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
@@ -756,269 +1253,269 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D13" s="7">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E13" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F13" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="G13" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H13" s="7">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="I13" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="J13" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M13" s="12">
-        <f t="shared" ref="M13:T13" si="5">(($A$14*3.7)/(C13*5))*0.75</f>
-        <v>10.101</v>
+        <f t="shared" ref="M13:T13" si="4">(($A$14*3.7)/(C13*5))*0.75</f>
+        <v>10.100999999999999</v>
       </c>
       <c r="N13" s="12">
-        <f t="shared" si="5"/>
-        <v>8.4175</v>
+        <f t="shared" si="4"/>
+        <v>8.4175000000000004</v>
       </c>
       <c r="O13" s="12">
-        <f t="shared" si="5"/>
-        <v>10.101</v>
+        <f t="shared" si="4"/>
+        <v>10.100999999999999</v>
       </c>
       <c r="P13" s="12">
-        <f t="shared" si="5"/>
-        <v>7.215</v>
+        <f t="shared" si="4"/>
+        <v>7.2149999999999999</v>
       </c>
       <c r="Q13" s="12">
-        <f t="shared" si="5"/>
-        <v>5.0505</v>
+        <f t="shared" si="4"/>
+        <v>5.0504999999999995</v>
       </c>
       <c r="R13" s="12">
-        <f t="shared" si="5"/>
-        <v>2.805833333</v>
+        <f t="shared" si="4"/>
+        <v>2.8058333333333332</v>
       </c>
       <c r="S13" s="12">
-        <f t="shared" si="5"/>
-        <v>4.39173913</v>
+        <f t="shared" si="4"/>
+        <v>4.3917391304347824</v>
       </c>
       <c r="T13" s="12">
-        <f t="shared" si="5"/>
-        <v>4.39173913</v>
-      </c>
-    </row>
-    <row r="14">
+        <f t="shared" si="4"/>
+        <v>4.3917391304347824</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
-        <v>1820.0</v>
+        <v>1820</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D14" s="7">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="E14" s="7">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="F14" s="7">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="G14" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H14" s="7">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="I14" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="J14" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="12">
-        <f t="shared" ref="M14:T14" si="6">(($A$14*3.7)/(C14*5))*0.75</f>
-        <v>7.215</v>
+        <f t="shared" ref="M14:T14" si="5">(($A$14*3.7)/(C14*5))*0.75</f>
+        <v>7.2149999999999999</v>
       </c>
       <c r="N14" s="12">
-        <f t="shared" si="6"/>
-        <v>6.313125</v>
+        <f t="shared" si="5"/>
+        <v>6.3131250000000003</v>
       </c>
       <c r="O14" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>7.77</v>
       </c>
       <c r="P14" s="12">
-        <f t="shared" si="6"/>
-        <v>5.316315789</v>
+        <f t="shared" si="5"/>
+        <v>5.3163157894736841</v>
       </c>
       <c r="Q14" s="12">
-        <f t="shared" si="6"/>
-        <v>4.39173913</v>
+        <f t="shared" si="5"/>
+        <v>4.3917391304347824</v>
       </c>
       <c r="R14" s="12">
-        <f t="shared" si="6"/>
-        <v>2.52525</v>
+        <f t="shared" si="5"/>
+        <v>2.5252499999999998</v>
       </c>
       <c r="S14" s="12">
-        <f t="shared" si="6"/>
-        <v>3.258387097</v>
+        <f t="shared" si="5"/>
+        <v>3.2583870967741939</v>
       </c>
       <c r="T14" s="12">
-        <f t="shared" si="6"/>
-        <v>3.258387097</v>
-      </c>
-    </row>
-    <row r="15">
+        <f t="shared" si="5"/>
+        <v>3.2583870967741939</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D15" s="7">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="E15" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="F15" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="G15" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H15" s="7">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="I15" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="J15" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M15" s="12">
-        <f t="shared" ref="M15:T15" si="7">(($A$14*3.7)/(C15*5))*0.75</f>
-        <v>7.215</v>
+        <f t="shared" ref="M15:T15" si="6">(($A$14*3.7)/(C15*5))*0.75</f>
+        <v>7.2149999999999999</v>
       </c>
       <c r="N15" s="12">
-        <f t="shared" si="7"/>
-        <v>5.941764706</v>
+        <f t="shared" si="6"/>
+        <v>5.9417647058823526</v>
       </c>
       <c r="O15" s="12">
-        <f t="shared" si="7"/>
-        <v>7.215</v>
+        <f t="shared" si="6"/>
+        <v>7.2149999999999999</v>
       </c>
       <c r="P15" s="12">
-        <f t="shared" si="7"/>
-        <v>5.0505</v>
+        <f t="shared" si="6"/>
+        <v>5.0504999999999995</v>
       </c>
       <c r="Q15" s="12">
-        <f t="shared" si="7"/>
-        <v>4.20875</v>
+        <f t="shared" si="6"/>
+        <v>4.2087500000000002</v>
       </c>
       <c r="R15" s="12">
-        <f t="shared" si="7"/>
-        <v>2.405</v>
+        <f t="shared" si="6"/>
+        <v>2.4049999999999998</v>
       </c>
       <c r="S15" s="12">
-        <f t="shared" si="7"/>
-        <v>3.483103448</v>
+        <f t="shared" si="6"/>
+        <v>3.4831034482758625</v>
       </c>
       <c r="T15" s="12">
-        <f t="shared" si="7"/>
-        <v>3.483103448</v>
-      </c>
-    </row>
-    <row r="16">
+        <f t="shared" si="6"/>
+        <v>3.4831034482758625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D16" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="E16" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F16" s="7">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="G16" s="7">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H16" s="7">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="I16" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="J16" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M16" s="12">
-        <f t="shared" ref="M16:T16" si="8">(($A$14*3.7)/(C16*5))*0.75</f>
-        <v>4.20875</v>
+        <f t="shared" ref="M16:T16" si="7">(($A$14*3.7)/(C16*5))*0.75</f>
+        <v>4.2087500000000002</v>
       </c>
       <c r="N16" s="12">
-        <f t="shared" si="8"/>
-        <v>4.39173913</v>
+        <f t="shared" si="7"/>
+        <v>4.3917391304347824</v>
       </c>
       <c r="O16" s="12">
-        <f t="shared" si="8"/>
-        <v>4.39173913</v>
+        <f t="shared" si="7"/>
+        <v>4.3917391304347824</v>
       </c>
       <c r="P16" s="12">
-        <f t="shared" si="8"/>
-        <v>3.1565625</v>
+        <f t="shared" si="7"/>
+        <v>3.1565625000000002</v>
       </c>
       <c r="Q16" s="12">
-        <f t="shared" si="8"/>
-        <v>3.060909091</v>
+        <f t="shared" si="7"/>
+        <v>3.0609090909090906</v>
       </c>
       <c r="R16" s="12">
-        <f t="shared" si="8"/>
-        <v>2.104375</v>
+        <f t="shared" si="7"/>
+        <v>2.1043750000000001</v>
       </c>
       <c r="S16" s="12">
-        <f t="shared" si="8"/>
-        <v>2.886</v>
+        <f t="shared" si="7"/>
+        <v>2.8860000000000001</v>
       </c>
       <c r="T16" s="12">
-        <f t="shared" si="8"/>
-        <v>2.886</v>
-      </c>
-    </row>
-    <row r="17">
+        <f t="shared" si="7"/>
+        <v>2.8860000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1035,7 +1532,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
@@ -1147,269 +1644,269 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D20" s="7">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E20" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F20" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="G20" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H20" s="7">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="I20" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="J20" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M20" s="12">
-        <f t="shared" ref="M20:T20" si="9">(($A$21*3.7)/(C20*5))*0.75</f>
-        <v>12.765</v>
+        <f t="shared" ref="M20:T20" si="8">(($A$21*3.7)/(C20*5))*0.75</f>
+        <v>12.765000000000001</v>
       </c>
       <c r="N20" s="12">
-        <f t="shared" si="9"/>
-        <v>10.6375</v>
+        <f t="shared" si="8"/>
+        <v>10.637499999999999</v>
       </c>
       <c r="O20" s="12">
-        <f t="shared" si="9"/>
-        <v>12.765</v>
+        <f t="shared" si="8"/>
+        <v>12.765000000000001</v>
       </c>
       <c r="P20" s="12">
-        <f t="shared" si="9"/>
-        <v>9.117857143</v>
+        <f t="shared" si="8"/>
+        <v>9.117857142857142</v>
       </c>
       <c r="Q20" s="12">
-        <f t="shared" si="9"/>
-        <v>6.3825</v>
+        <f t="shared" si="8"/>
+        <v>6.3825000000000003</v>
       </c>
       <c r="R20" s="12">
-        <f t="shared" si="9"/>
-        <v>3.545833333</v>
+        <f t="shared" si="8"/>
+        <v>3.5458333333333334</v>
       </c>
       <c r="S20" s="12">
-        <f t="shared" si="9"/>
-        <v>5.55</v>
+        <f t="shared" si="8"/>
+        <v>5.5500000000000007</v>
       </c>
       <c r="T20" s="12">
-        <f t="shared" si="9"/>
-        <v>5.55</v>
-      </c>
-    </row>
-    <row r="21">
+        <f t="shared" si="8"/>
+        <v>5.5500000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <v>2300.0</v>
+        <v>2300</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D21" s="7">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="E21" s="7">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="F21" s="7">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="G21" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H21" s="7">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="I21" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="J21" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M21" s="12">
-        <f t="shared" ref="M21:T21" si="10">(($A$21*3.7)/(C21*5))*0.75</f>
-        <v>9.117857143</v>
+        <f t="shared" ref="M21:T21" si="9">(($A$21*3.7)/(C21*5))*0.75</f>
+        <v>9.117857142857142</v>
       </c>
       <c r="N21" s="12">
-        <f t="shared" si="10"/>
-        <v>7.978125</v>
+        <f t="shared" si="9"/>
+        <v>7.9781249999999995</v>
       </c>
       <c r="O21" s="12">
-        <f t="shared" si="10"/>
-        <v>9.819230769</v>
+        <f t="shared" si="9"/>
+        <v>9.819230769230769</v>
       </c>
       <c r="P21" s="12">
-        <f t="shared" si="10"/>
-        <v>6.718421053</v>
+        <f t="shared" si="9"/>
+        <v>6.7184210526315784</v>
       </c>
       <c r="Q21" s="12">
-        <f t="shared" si="10"/>
-        <v>5.55</v>
+        <f t="shared" si="9"/>
+        <v>5.5500000000000007</v>
       </c>
       <c r="R21" s="12">
-        <f t="shared" si="10"/>
-        <v>3.19125</v>
+        <f t="shared" si="9"/>
+        <v>3.1912500000000001</v>
       </c>
       <c r="S21" s="12">
-        <f t="shared" si="10"/>
-        <v>4.117741935</v>
+        <f t="shared" si="9"/>
+        <v>4.1177419354838705</v>
       </c>
       <c r="T21" s="12">
-        <f t="shared" si="10"/>
-        <v>4.117741935</v>
-      </c>
-    </row>
-    <row r="22">
+        <f t="shared" si="9"/>
+        <v>4.1177419354838705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D22" s="7">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="E22" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="F22" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="G22" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H22" s="7">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="I22" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="J22" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M22" s="12">
-        <f t="shared" ref="M22:T22" si="11">(($A$21*3.7)/(C22*5))*0.75</f>
-        <v>9.117857143</v>
+        <f t="shared" ref="M22:T22" si="10">(($A$21*3.7)/(C22*5))*0.75</f>
+        <v>9.117857142857142</v>
       </c>
       <c r="N22" s="12">
-        <f t="shared" si="11"/>
-        <v>7.508823529</v>
+        <f t="shared" si="10"/>
+        <v>7.5088235294117647</v>
       </c>
       <c r="O22" s="12">
-        <f t="shared" si="11"/>
-        <v>9.117857143</v>
+        <f t="shared" si="10"/>
+        <v>9.117857142857142</v>
       </c>
       <c r="P22" s="12">
-        <f t="shared" si="11"/>
-        <v>6.3825</v>
+        <f t="shared" si="10"/>
+        <v>6.3825000000000003</v>
       </c>
       <c r="Q22" s="12">
-        <f t="shared" si="11"/>
-        <v>5.31875</v>
+        <f t="shared" si="10"/>
+        <v>5.3187499999999996</v>
       </c>
       <c r="R22" s="12">
-        <f t="shared" si="11"/>
-        <v>3.039285714</v>
+        <f t="shared" si="10"/>
+        <v>3.0392857142857141</v>
       </c>
       <c r="S22" s="12">
-        <f t="shared" si="11"/>
-        <v>4.401724138</v>
+        <f t="shared" si="10"/>
+        <v>4.4017241379310352</v>
       </c>
       <c r="T22" s="12">
-        <f t="shared" si="11"/>
-        <v>4.401724138</v>
-      </c>
-    </row>
-    <row r="23">
+        <f t="shared" si="10"/>
+        <v>4.4017241379310352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D23" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="E23" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F23" s="7">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="G23" s="7">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H23" s="7">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="I23" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="J23" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M23" s="12">
-        <f t="shared" ref="M23:T23" si="12">(($A$21*3.7)/(C23*5))*0.75</f>
-        <v>5.31875</v>
+        <f t="shared" ref="M23:T23" si="11">(($A$21*3.7)/(C23*5))*0.75</f>
+        <v>5.3187499999999996</v>
       </c>
       <c r="N23" s="12">
-        <f t="shared" si="12"/>
-        <v>5.55</v>
+        <f t="shared" si="11"/>
+        <v>5.5500000000000007</v>
       </c>
       <c r="O23" s="12">
-        <f t="shared" si="12"/>
-        <v>5.55</v>
+        <f t="shared" si="11"/>
+        <v>5.5500000000000007</v>
       </c>
       <c r="P23" s="12">
-        <f t="shared" si="12"/>
-        <v>3.9890625</v>
+        <f t="shared" si="11"/>
+        <v>3.9890624999999997</v>
       </c>
       <c r="Q23" s="12">
-        <f t="shared" si="12"/>
-        <v>3.868181818</v>
+        <f t="shared" si="11"/>
+        <v>3.8681818181818182</v>
       </c>
       <c r="R23" s="12">
-        <f t="shared" si="12"/>
-        <v>2.659375</v>
+        <f t="shared" si="11"/>
+        <v>2.6593749999999998</v>
       </c>
       <c r="S23" s="12">
-        <f t="shared" si="12"/>
-        <v>3.647142857</v>
+        <f t="shared" si="11"/>
+        <v>3.6471428571428572</v>
       </c>
       <c r="T23" s="12">
-        <f t="shared" si="12"/>
-        <v>3.647142857</v>
-      </c>
-    </row>
-    <row r="24">
+        <f t="shared" si="11"/>
+        <v>3.6471428571428572</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1426,7 +1923,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>0</v>
       </c>
@@ -1485,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7" t="s">
@@ -1538,269 +2035,269 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D27" s="7">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E27" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F27" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="G27" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H27" s="7">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="I27" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="J27" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M27" s="14">
-        <f t="shared" ref="M27:T27" si="13">(($A$28*3.7)/(C27*5))*0.75</f>
+        <f t="shared" ref="M27:T27" si="12">(($A$28*3.7)/(C27*5))*0.75</f>
         <v>27.75</v>
       </c>
       <c r="N27" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>23.125</v>
       </c>
       <c r="O27" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>27.75</v>
       </c>
       <c r="P27" s="14">
-        <f t="shared" si="13"/>
-        <v>19.82142857</v>
+        <f t="shared" si="12"/>
+        <v>19.821428571428569</v>
       </c>
       <c r="Q27" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>13.875</v>
       </c>
       <c r="R27" s="14">
-        <f t="shared" si="13"/>
-        <v>7.708333333</v>
+        <f t="shared" si="12"/>
+        <v>7.7083333333333339</v>
       </c>
       <c r="S27" s="14">
-        <f t="shared" si="13"/>
-        <v>12.06521739</v>
+        <f t="shared" si="12"/>
+        <v>12.065217391304348</v>
       </c>
       <c r="T27" s="14">
-        <f t="shared" si="13"/>
-        <v>12.06521739</v>
-      </c>
-    </row>
-    <row r="28">
+        <f t="shared" si="12"/>
+        <v>12.065217391304348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D28" s="7">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="E28" s="7">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="F28" s="7">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="G28" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H28" s="7">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="I28" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="J28" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M28" s="14">
-        <f t="shared" ref="M28:T28" si="14">(($A$28*3.7)/(C28*5))*0.75</f>
-        <v>19.82142857</v>
+        <f t="shared" ref="M28:T28" si="13">(($A$28*3.7)/(C28*5))*0.75</f>
+        <v>19.821428571428569</v>
       </c>
       <c r="N28" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>17.34375</v>
       </c>
       <c r="O28" s="14">
-        <f t="shared" si="14"/>
-        <v>21.34615385</v>
+        <f t="shared" si="13"/>
+        <v>21.346153846153847</v>
       </c>
       <c r="P28" s="14">
-        <f t="shared" si="14"/>
-        <v>14.60526316</v>
+        <f t="shared" si="13"/>
+        <v>14.605263157894736</v>
       </c>
       <c r="Q28" s="14">
-        <f t="shared" si="14"/>
-        <v>12.06521739</v>
+        <f t="shared" si="13"/>
+        <v>12.065217391304348</v>
       </c>
       <c r="R28" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>6.9375</v>
       </c>
       <c r="S28" s="14">
-        <f t="shared" si="14"/>
-        <v>8.951612903</v>
+        <f t="shared" si="13"/>
+        <v>8.9516129032258061</v>
       </c>
       <c r="T28" s="14">
-        <f t="shared" si="14"/>
-        <v>8.951612903</v>
-      </c>
-    </row>
-    <row r="29">
+        <f t="shared" si="13"/>
+        <v>8.9516129032258061</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D29" s="7">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="E29" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="F29" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="G29" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H29" s="7">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="I29" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="J29" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M29" s="14">
-        <f t="shared" ref="M29:T29" si="15">(($A$28*3.7)/(C29*5))*0.75</f>
-        <v>19.82142857</v>
+        <f t="shared" ref="M29:T29" si="14">(($A$28*3.7)/(C29*5))*0.75</f>
+        <v>19.821428571428569</v>
       </c>
       <c r="N29" s="14">
-        <f t="shared" si="15"/>
-        <v>16.32352941</v>
+        <f t="shared" si="14"/>
+        <v>16.323529411764707</v>
       </c>
       <c r="O29" s="14">
-        <f t="shared" si="15"/>
-        <v>19.82142857</v>
+        <f t="shared" si="14"/>
+        <v>19.821428571428569</v>
       </c>
       <c r="P29" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>13.875</v>
       </c>
       <c r="Q29" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>11.5625</v>
       </c>
       <c r="R29" s="14">
-        <f t="shared" si="15"/>
-        <v>6.607142857</v>
+        <f t="shared" si="14"/>
+        <v>6.6071428571428577</v>
       </c>
       <c r="S29" s="14">
-        <f t="shared" si="15"/>
-        <v>9.568965517</v>
+        <f t="shared" si="14"/>
+        <v>9.568965517241379</v>
       </c>
       <c r="T29" s="14">
-        <f t="shared" si="15"/>
-        <v>9.568965517</v>
-      </c>
-    </row>
-    <row r="30">
+        <f t="shared" si="14"/>
+        <v>9.568965517241379</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D30" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="E30" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F30" s="7">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="G30" s="7">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H30" s="7">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="I30" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="J30" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M30" s="14">
-        <f t="shared" ref="M30:T30" si="16">(($A$28*3.7)/(C30*5))*0.75</f>
+        <f t="shared" ref="M30:T30" si="15">(($A$28*3.7)/(C30*5))*0.75</f>
         <v>11.5625</v>
       </c>
       <c r="N30" s="14">
-        <f t="shared" si="16"/>
-        <v>12.06521739</v>
+        <f t="shared" si="15"/>
+        <v>12.065217391304348</v>
       </c>
       <c r="O30" s="14">
-        <f t="shared" si="16"/>
-        <v>12.06521739</v>
+        <f t="shared" si="15"/>
+        <v>12.065217391304348</v>
       </c>
       <c r="P30" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.671875</v>
       </c>
       <c r="Q30" s="14">
-        <f t="shared" si="16"/>
-        <v>8.409090909</v>
+        <f t="shared" si="15"/>
+        <v>8.4090909090909101</v>
       </c>
       <c r="R30" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>5.78125</v>
       </c>
       <c r="S30" s="14">
-        <f t="shared" si="16"/>
-        <v>7.928571429</v>
+        <f t="shared" si="15"/>
+        <v>7.9285714285714288</v>
       </c>
       <c r="T30" s="14">
-        <f t="shared" si="16"/>
-        <v>7.928571429</v>
-      </c>
-    </row>
-    <row r="32">
+        <f t="shared" si="15"/>
+        <v>7.9285714285714288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +2356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7" t="s">
@@ -1912,269 +2409,270 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="D34" s="7">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="E34" s="7">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F34" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="G34" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H34" s="7">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="I34" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="J34" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" ref="M34:T34" si="17">(($A$35*3.7)/(C34*5))*0.75</f>
-        <v>66.6</v>
+        <f t="shared" ref="M34:T34" si="16">(($A$35*3.7)/(C34*5))*0.75</f>
+        <v>66.599999999999994</v>
       </c>
       <c r="N34" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>55.5</v>
       </c>
       <c r="O34" s="9">
-        <f t="shared" si="17"/>
-        <v>66.6</v>
+        <f t="shared" si="16"/>
+        <v>66.599999999999994</v>
       </c>
       <c r="P34" s="9">
-        <f t="shared" si="17"/>
-        <v>47.57142857</v>
+        <f t="shared" si="16"/>
+        <v>47.571428571428569</v>
       </c>
       <c r="Q34" s="9">
-        <f t="shared" si="17"/>
-        <v>33.3</v>
+        <f t="shared" si="16"/>
+        <v>33.299999999999997</v>
       </c>
       <c r="R34" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>18.5</v>
       </c>
       <c r="S34" s="9">
-        <f t="shared" si="17"/>
-        <v>28.95652174</v>
+        <f t="shared" si="16"/>
+        <v>28.956521739130437</v>
       </c>
       <c r="T34" s="9">
-        <f t="shared" si="17"/>
-        <v>28.95652174</v>
-      </c>
-    </row>
-    <row r="35">
+        <f t="shared" si="16"/>
+        <v>28.956521739130437</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
-        <v>12000.0</v>
+        <v>12000</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D35" s="7">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="E35" s="7">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="F35" s="7">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="G35" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="H35" s="7">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="I35" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="J35" s="7">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="M35" s="9">
-        <f t="shared" ref="M35:T35" si="18">(($A$35*3.7)/(C35*5))*0.75</f>
-        <v>47.57142857</v>
+        <f t="shared" ref="M35:T35" si="17">(($A$35*3.7)/(C35*5))*0.75</f>
+        <v>47.571428571428569</v>
       </c>
       <c r="N35" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>41.625</v>
       </c>
       <c r="O35" s="9">
-        <f t="shared" si="18"/>
-        <v>51.23076923</v>
+        <f t="shared" si="17"/>
+        <v>51.230769230769226</v>
       </c>
       <c r="P35" s="9">
-        <f t="shared" si="18"/>
-        <v>35.05263158</v>
+        <f t="shared" si="17"/>
+        <v>35.05263157894737</v>
       </c>
       <c r="Q35" s="9">
-        <f t="shared" si="18"/>
-        <v>28.95652174</v>
+        <f t="shared" si="17"/>
+        <v>28.956521739130437</v>
       </c>
       <c r="R35" s="9">
-        <f t="shared" si="18"/>
-        <v>16.65</v>
+        <f t="shared" si="17"/>
+        <v>16.649999999999999</v>
       </c>
       <c r="S35" s="9">
-        <f t="shared" si="18"/>
-        <v>21.48387097</v>
+        <f t="shared" si="17"/>
+        <v>21.483870967741936</v>
       </c>
       <c r="T35" s="9">
-        <f t="shared" si="18"/>
-        <v>21.48387097</v>
-      </c>
-    </row>
-    <row r="36">
+        <f t="shared" si="17"/>
+        <v>21.483870967741936</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="D36" s="7">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="E36" s="7">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="F36" s="7">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="G36" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="H36" s="7">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="I36" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="J36" s="7">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M36" s="9">
-        <f t="shared" ref="M36:T36" si="19">(($A$35*3.7)/(C36*5))*0.75</f>
-        <v>47.57142857</v>
+        <f t="shared" ref="M36:T36" si="18">(($A$35*3.7)/(C36*5))*0.75</f>
+        <v>47.571428571428569</v>
       </c>
       <c r="N36" s="9">
-        <f t="shared" si="19"/>
-        <v>39.17647059</v>
+        <f t="shared" si="18"/>
+        <v>39.17647058823529</v>
       </c>
       <c r="O36" s="9">
-        <f t="shared" si="19"/>
-        <v>47.57142857</v>
+        <f t="shared" si="18"/>
+        <v>47.571428571428569</v>
       </c>
       <c r="P36" s="9">
-        <f t="shared" si="19"/>
-        <v>33.3</v>
+        <f t="shared" si="18"/>
+        <v>33.299999999999997</v>
       </c>
       <c r="Q36" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>27.75</v>
       </c>
       <c r="R36" s="9">
-        <f t="shared" si="19"/>
-        <v>15.85714286</v>
+        <f t="shared" si="18"/>
+        <v>15.857142857142858</v>
       </c>
       <c r="S36" s="9">
-        <f t="shared" si="19"/>
-        <v>22.96551724</v>
+        <f t="shared" si="18"/>
+        <v>22.96551724137931</v>
       </c>
       <c r="T36" s="9">
-        <f t="shared" si="19"/>
-        <v>22.96551724</v>
-      </c>
-    </row>
-    <row r="37">
+        <f t="shared" si="18"/>
+        <v>22.96551724137931</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="7">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D37" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="E37" s="7">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F37" s="7">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="G37" s="7">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="H37" s="7">
-        <v>480.0</v>
+        <v>480</v>
       </c>
       <c r="I37" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="J37" s="7">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" ref="M37:T37" si="20">(($A$35*3.7)/(C37*5))*0.75</f>
+        <f t="shared" ref="M37:T37" si="19">(($A$35*3.7)/(C37*5))*0.75</f>
         <v>27.75</v>
       </c>
       <c r="N37" s="9">
-        <f t="shared" si="20"/>
-        <v>28.95652174</v>
+        <f t="shared" si="19"/>
+        <v>28.956521739130437</v>
       </c>
       <c r="O37" s="9">
-        <f t="shared" si="20"/>
-        <v>28.95652174</v>
+        <f t="shared" si="19"/>
+        <v>28.956521739130437</v>
       </c>
       <c r="P37" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>20.8125</v>
       </c>
       <c r="Q37" s="9">
-        <f t="shared" si="20"/>
-        <v>20.18181818</v>
+        <f t="shared" si="19"/>
+        <v>20.181818181818183</v>
       </c>
       <c r="R37" s="9">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>13.875</v>
       </c>
       <c r="S37" s="9">
-        <f t="shared" si="20"/>
-        <v>19.02857143</v>
+        <f t="shared" si="19"/>
+        <v>19.028571428571428</v>
       </c>
       <c r="T37" s="9">
-        <f t="shared" si="20"/>
-        <v>19.02857143</v>
+        <f t="shared" si="19"/>
+        <v>19.028571428571428</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>